<commit_message>
Added charts tests to admin dash
</commit_message>
<xml_diff>
--- a/cypress/downloads/Hubzity_-_Account_stats_for_Patternz.xlsx
+++ b/cypress/downloads/Hubzity_-_Account_stats_for_Patternz.xlsx
@@ -420,16 +420,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>campaign_jCiEsmQGldMt4a2nER9k3N5zkpVwb</v>
+        <v>campaign_fFLML21TlvlGAzHlw3SLlHv0difPft</v>
       </c>
       <c r="B2" t="str">
-        <v>ACTIVE</v>
+        <v>INACTIVE</v>
       </c>
       <c r="C2" t="str">
-        <v>mouse</v>
+        <v>play</v>
       </c>
       <c r="D2">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -458,25 +458,25 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>campaign_fFLML21TlvlGAzHlw3SLlHv0difPft</v>
+        <v>campaign_jCiEsmQGldMt4a2nER9k3N5zkpVwb</v>
       </c>
       <c r="B3" t="str">
-        <v>ACTIVE</v>
+        <v>INACTIVE</v>
       </c>
       <c r="C3" t="str">
-        <v>play</v>
+        <v>mouse</v>
       </c>
       <c r="D3">
-        <v>966</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" t="str">
-        <v>0.9</v>
+        <v>0.0</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -485,10 +485,10 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.93</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>2.07</v>
+        <v>0</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -496,40 +496,40 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>campaign_1oCXpGca51PKrrEPfbIflkqPdSXi</v>
+        <v>campaign_Hk5mBwb0NxvbzVPiCvlDw7ATXaCAs3</v>
       </c>
       <c r="B4" t="str">
         <v>INACTIVE</v>
       </c>
       <c r="C4" t="str">
-        <v>Mexico casino</v>
+        <v>roladin</v>
       </c>
       <c r="D4">
-        <v>44622</v>
+        <v>6</v>
       </c>
       <c r="E4">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="G4" t="str">
-        <v>44.5</v>
+        <v>0.0</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0.82</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>0.24</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start of Exchanges section testing
</commit_message>
<xml_diff>
--- a/cypress/downloads/Hubzity_-_Account_stats_for_Patternz.xlsx
+++ b/cypress/downloads/Hubzity_-_Account_stats_for_Patternz.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -384,157 +384,10 @@
       <c r="A1" t="str">
         <v>Campaign ID</v>
       </c>
-      <c r="B1" t="str">
-        <v>Campaign Status</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Campaign Name</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Impressions</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Clicks</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Conversions</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Cost</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Payout</v>
-      </c>
-      <c r="I1" t="str">
-        <v>eCPI</v>
-      </c>
-      <c r="J1" t="str">
-        <v>eCPM</v>
-      </c>
-      <c r="K1" t="str">
-        <v>CTR</v>
-      </c>
-      <c r="L1" t="str">
-        <v>CR</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>campaign_fFLML21TlvlGAzHlw3SLlHv0difPft</v>
-      </c>
-      <c r="B2" t="str">
-        <v>INACTIVE</v>
-      </c>
-      <c r="C2" t="str">
-        <v>play</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="str">
-        <v>0.0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>campaign_jCiEsmQGldMt4a2nER9k3N5zkpVwb</v>
-      </c>
-      <c r="B3" t="str">
-        <v>INACTIVE</v>
-      </c>
-      <c r="C3" t="str">
-        <v>mouse</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" t="str">
-        <v>0.0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>campaign_Hk5mBwb0NxvbzVPiCvlDw7ATXaCAs3</v>
-      </c>
-      <c r="B4" t="str">
-        <v>INACTIVE</v>
-      </c>
-      <c r="C4" t="str">
-        <v>roladin</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" t="str">
-        <v>0.0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>